<commit_message>
Changed gitignore to ignore excel files
</commit_message>
<xml_diff>
--- a/Class Work/CS 2318/Assignment Optional 1/AssignOpt01_StackFrameDetails.xlsx
+++ b/Class Work/CS 2318/Assignment Optional 1/AssignOpt01_StackFrameDetails.xlsx
@@ -5,18 +5,20 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lk04\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndela\Documents\Code Workspace\School-Work\Class Work\CS 2318\Assignment Optional 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F063FC94-1FB4-46AB-B36D-70D0AECC493C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1934B8D0-1DF1-4C99-A87F-2741F7DD390A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13185" yWindow="4620" windowWidth="15345" windowHeight="10980" tabRatio="875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="5" r:id="rId1"/>
     <sheet name="CoutCstrNL" sheetId="20" r:id="rId2"/>
     <sheet name="PopulateArray" sheetId="22" r:id="rId3"/>
     <sheet name="ShowArrayLabeled" sheetId="9" r:id="rId4"/>
+    <sheet name="hasDup" sheetId="24" r:id="rId5"/>
+    <sheet name="Exists" sheetId="25" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">CoutCstrNL!$A$1:$AB$59</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="71">
   <si>
     <t>SP (old)</t>
   </si>
@@ -252,6 +254,24 @@
   <si>
     <t>'+'</t>
   </si>
+  <si>
+    <t>($fP)</t>
+  </si>
+  <si>
+    <t>numEle</t>
+  </si>
+  <si>
+    <t>arrBegPtr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show </t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>($ra)</t>
+  </si>
 </sst>
 </file>
 
@@ -382,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -516,6 +536,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2598,6 +2633,122 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>986</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2E14801-3166-4BA1-B09C-E28BFB8310B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1476375" y="13030200"/>
+          <a:ext cx="180975" cy="986"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>986</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B164FD7A-791A-439A-9D32-5B78D94AB045}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1219200" y="13382625"/>
+          <a:ext cx="180975" cy="986"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2924,7 +3075,9 @@
   </sheetPr>
   <dimension ref="A2:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4759,7 +4912,9 @@
   </sheetPr>
   <dimension ref="A2:AB56"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6195,17 +6350,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AB16:AB17"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="Y31:Y32"/>
+    <mergeCell ref="Y37:Y38"/>
     <mergeCell ref="D54:D55"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B47:B50"/>
     <mergeCell ref="B51:B54"/>
-    <mergeCell ref="AB16:AB17"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="Y31:Y32"/>
-    <mergeCell ref="Y37:Y38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
@@ -6224,7 +6379,9 @@
   </sheetPr>
   <dimension ref="A2:AB56"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8057,9 +8214,11 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AB56"/>
+  <dimension ref="A1:AB56"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView topLeftCell="A22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8085,6 +8244,11 @@
     <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="G2" s="9"/>
@@ -9515,4 +9679,858 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF87040-F013-4F9A-9DBB-EA8AF4DA35C3}">
+  <dimension ref="A3:D55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="12"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>47</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>46</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>45</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>44</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>43</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>42</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>41</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>40</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>39</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>38</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>37</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>35</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>34</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>33</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>32</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="D22" s="47"/>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>31</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>30</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>29</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>28</v>
+      </c>
+      <c r="B26" s="44"/>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>27</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>26</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="16">
+        <v>25</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>24</v>
+      </c>
+      <c r="B30" s="44"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>23</v>
+      </c>
+      <c r="B31" s="48"/>
+      <c r="D31" s="47"/>
+    </row>
+    <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>22</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="D32" s="47"/>
+    </row>
+    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <v>21</v>
+      </c>
+      <c r="B33" s="49"/>
+      <c r="D33" s="47"/>
+    </row>
+    <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <v>20</v>
+      </c>
+      <c r="B34" s="49"/>
+      <c r="D34" s="47"/>
+    </row>
+    <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>19</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="D35" s="47"/>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
+        <v>18</v>
+      </c>
+      <c r="B36" s="49"/>
+      <c r="D36" s="47"/>
+    </row>
+    <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="16">
+        <v>17</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="D37" s="47"/>
+    </row>
+    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>16</v>
+      </c>
+      <c r="B38" s="50"/>
+      <c r="D38" s="47"/>
+    </row>
+    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>15</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
+        <v>14</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="16">
+        <v>13</v>
+      </c>
+      <c r="B41" s="46"/>
+      <c r="D41" s="35"/>
+    </row>
+    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
+        <v>12</v>
+      </c>
+      <c r="B42" s="44"/>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
+        <v>11</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
+        <v>10</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="16">
+        <v>9</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>8</v>
+      </c>
+      <c r="B46" s="44"/>
+      <c r="D46" s="35"/>
+    </row>
+    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
+        <v>7</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>6</v>
+      </c>
+      <c r="B48" s="46"/>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>5</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>4</v>
+      </c>
+      <c r="B50" s="44"/>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>3</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>2</v>
+      </c>
+      <c r="B52" s="46"/>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>1</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>0</v>
+      </c>
+      <c r="B54" s="44"/>
+      <c r="D54" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
+      <c r="B55" s="3"/>
+      <c r="D55" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC24030D-97E3-4514-B85B-2E3B2267588F}">
+  <dimension ref="A3:G55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="12"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>47</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>46</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>45</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>44</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>43</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>42</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>41</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>40</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>39</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>38</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>37</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>35</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>34</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>33</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>32</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="D22" s="47"/>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>31</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>30</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>29</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>28</v>
+      </c>
+      <c r="B26" s="44"/>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>27</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>26</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="16">
+        <v>25</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>24</v>
+      </c>
+      <c r="B30" s="44"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>23</v>
+      </c>
+      <c r="B31" s="48"/>
+      <c r="D31" s="47"/>
+    </row>
+    <row r="32" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>22</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="D32" s="47"/>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <v>21</v>
+      </c>
+      <c r="B33" s="49"/>
+      <c r="D33" s="47"/>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <v>20</v>
+      </c>
+      <c r="B34" s="49"/>
+      <c r="D34" s="47"/>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>19</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="D35" s="47"/>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
+        <v>18</v>
+      </c>
+      <c r="B36" s="49"/>
+      <c r="D36" s="47"/>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="16">
+        <v>17</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="D37" s="47"/>
+    </row>
+    <row r="38" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>16</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="D38" s="47"/>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>15</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
+        <v>14</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="16">
+        <v>13</v>
+      </c>
+      <c r="B41" s="46"/>
+      <c r="D41" s="35"/>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
+        <v>12</v>
+      </c>
+      <c r="B42" s="44"/>
+      <c r="D42" s="35"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
+        <v>11</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
+        <v>10</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="D44" s="35"/>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="16">
+        <v>9</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>8</v>
+      </c>
+      <c r="B46" s="44"/>
+      <c r="D46" s="35"/>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
+        <v>7</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>6</v>
+      </c>
+      <c r="B48" s="46"/>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>5</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="D49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>4</v>
+      </c>
+      <c r="B50" s="44"/>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>3</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>2</v>
+      </c>
+      <c r="B52" s="46"/>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>1</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>0</v>
+      </c>
+      <c r="B54" s="44"/>
+      <c r="D54" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
+      <c r="B55" s="3"/>
+      <c r="D55" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="D23:D26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>